<commit_message>
Inclusão dos outros cenários nos arquivos de manutenção e de ordens.
</commit_message>
<xml_diff>
--- a/inputs/dataset_maquinas.xlsx
+++ b/inputs/dataset_maquinas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Production_Scheduling_RL\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E62C51-F5D2-457C-8920-55B415147B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B90B0-75B2-4270-97F5-7681B9855AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{123EE8DF-F984-4E7E-8A09-7256808DEDFD}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>29660</v>
+        <v>6345</v>
       </c>
       <c r="C2">
         <v>673</v>
@@ -647,7 +647,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>44537</v>
+        <v>2129</v>
       </c>
       <c r="C3">
         <v>644</v>
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>23008</v>
+        <v>5608</v>
       </c>
       <c r="C4">
         <v>715</v>
@@ -675,7 +675,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>59606</v>
+        <v>1736</v>
       </c>
       <c r="C5">
         <v>840</v>
@@ -689,7 +689,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>70475</v>
+        <v>2389</v>
       </c>
       <c r="C6">
         <v>641</v>
@@ -703,7 +703,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>68253</v>
+        <v>5064</v>
       </c>
       <c r="C7">
         <v>835</v>
@@ -717,7 +717,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>64853</v>
+        <v>8016</v>
       </c>
       <c r="C8">
         <v>663</v>
@@ -731,7 +731,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>57910</v>
+        <v>7658</v>
       </c>
       <c r="C9">
         <v>747</v>
@@ -745,7 +745,7 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>47410</v>
+        <v>5231</v>
       </c>
       <c r="C10">
         <v>702</v>
@@ -759,7 +759,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>34882</v>
+        <v>2548</v>
       </c>
       <c r="C11">
         <v>859</v>
@@ -773,7 +773,7 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>50336</v>
+        <v>3524</v>
       </c>
       <c r="C12">
         <v>686</v>
@@ -787,7 +787,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>41357</v>
+        <v>8345</v>
       </c>
       <c r="C13">
         <v>750</v>
@@ -801,7 +801,7 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>36443</v>
+        <v>7770</v>
       </c>
       <c r="C14">
         <v>805</v>
@@ -815,7 +815,7 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>24133</v>
+        <v>5737</v>
       </c>
       <c r="C15">
         <v>854</v>
@@ -829,7 +829,7 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>26950</v>
+        <v>8035</v>
       </c>
       <c r="C16">
         <v>745</v>
@@ -843,7 +843,7 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>61642</v>
+        <v>4638</v>
       </c>
       <c r="C17">
         <v>792</v>
@@ -857,7 +857,7 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>41573</v>
+        <v>9459</v>
       </c>
       <c r="C18">
         <v>793</v>
@@ -871,7 +871,7 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>63800</v>
+        <v>3013</v>
       </c>
       <c r="C19">
         <v>842</v>
@@ -885,7 +885,7 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>63214</v>
+        <v>4781</v>
       </c>
       <c r="C20">
         <v>715</v>
@@ -899,7 +899,7 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>69461</v>
+        <v>2677</v>
       </c>
       <c r="C21">
         <v>648</v>
@@ -913,7 +913,7 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>36360</v>
+        <v>5606</v>
       </c>
       <c r="C22">
         <v>736</v>
@@ -927,7 +927,7 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>57006</v>
+        <v>3848</v>
       </c>
       <c r="C23">
         <v>723</v>
@@ -941,7 +941,7 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>63344</v>
+        <v>4980</v>
       </c>
       <c r="C24">
         <v>657</v>
@@ -955,7 +955,7 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>35627</v>
+        <v>8304</v>
       </c>
       <c r="C25">
         <v>711</v>
@@ -969,7 +969,7 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>69988</v>
+        <v>8098</v>
       </c>
       <c r="C26">
         <v>796</v>
@@ -983,7 +983,7 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>53451</v>
+        <v>4222</v>
       </c>
       <c r="C27">
         <v>724</v>
@@ -997,7 +997,7 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>70189</v>
+        <v>9827</v>
       </c>
       <c r="C28">
         <v>711</v>
@@ -1011,7 +1011,7 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>70001</v>
+        <v>6381</v>
       </c>
       <c r="C29">
         <v>877</v>
@@ -1025,7 +1025,7 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>56882</v>
+        <v>6600</v>
       </c>
       <c r="C30">
         <v>745</v>
@@ -1039,7 +1039,7 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>33603</v>
+        <v>3076</v>
       </c>
       <c r="C31">
         <v>780</v>
@@ -1053,7 +1053,7 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>29146</v>
+        <v>7835</v>
       </c>
       <c r="C32">
         <v>708</v>
@@ -1067,7 +1067,7 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>55396</v>
+        <v>6582</v>
       </c>
       <c r="C33">
         <v>829</v>
@@ -1081,7 +1081,7 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>28353</v>
+        <v>3727</v>
       </c>
       <c r="C34">
         <v>605</v>
@@ -1095,7 +1095,7 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>55623</v>
+        <v>6906</v>
       </c>
       <c r="C35">
         <v>705</v>
@@ -1109,7 +1109,7 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>44326</v>
+        <v>2857</v>
       </c>
       <c r="C36">
         <v>783</v>
@@ -1123,7 +1123,7 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>50472</v>
+        <v>9265</v>
       </c>
       <c r="C37">
         <v>629</v>
@@ -1137,7 +1137,7 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>53406</v>
+        <v>2619</v>
       </c>
       <c r="C38">
         <v>730</v>
@@ -1151,7 +1151,7 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>40978</v>
+        <v>6902</v>
       </c>
       <c r="C39">
         <v>783</v>
@@ -1165,7 +1165,7 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>59474</v>
+        <v>9409</v>
       </c>
       <c r="C40">
         <v>826</v>
@@ -1179,7 +1179,7 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>59220</v>
+        <v>2810</v>
       </c>
       <c r="C41">
         <v>652</v>
@@ -1193,7 +1193,7 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>45475</v>
+        <v>4858</v>
       </c>
       <c r="C42">
         <v>695</v>
@@ -1207,7 +1207,7 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>48120</v>
+        <v>6426</v>
       </c>
       <c r="C43">
         <v>656</v>
@@ -1221,7 +1221,7 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>47730</v>
+        <v>9777</v>
       </c>
       <c r="C44">
         <v>805</v>
@@ -1235,7 +1235,7 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>52062</v>
+        <v>4073</v>
       </c>
       <c r="C45">
         <v>872</v>
@@ -1249,7 +1249,7 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>49128</v>
+        <v>4622</v>
       </c>
       <c r="C46">
         <v>827</v>
@@ -1263,7 +1263,7 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>59570</v>
+        <v>5128</v>
       </c>
       <c r="C47">
         <v>871</v>
@@ -1277,7 +1277,7 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>34547</v>
+        <v>4733</v>
       </c>
       <c r="C48">
         <v>652</v>
@@ -1291,7 +1291,7 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>46404</v>
+        <v>2041</v>
       </c>
       <c r="C49">
         <v>620</v>
@@ -1305,7 +1305,7 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>70183</v>
+        <v>9603</v>
       </c>
       <c r="C50">
         <v>698</v>
@@ -1319,7 +1319,7 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>47747</v>
+        <v>9591</v>
       </c>
       <c r="C51">
         <v>791</v>
@@ -1333,7 +1333,7 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>57579</v>
+        <v>5738</v>
       </c>
       <c r="C52">
         <v>805</v>
@@ -1347,7 +1347,7 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>59991</v>
+        <v>6548</v>
       </c>
       <c r="C53">
         <v>788</v>
@@ -1361,7 +1361,7 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>21613</v>
+        <v>9995</v>
       </c>
       <c r="C54">
         <v>695</v>
@@ -1375,7 +1375,7 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>57140</v>
+        <v>2633</v>
       </c>
       <c r="C55">
         <v>707</v>
@@ -1389,7 +1389,7 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>23892</v>
+        <v>5667</v>
       </c>
       <c r="C56">
         <v>695</v>
@@ -1403,7 +1403,7 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>62122</v>
+        <v>3343</v>
       </c>
       <c r="C57">
         <v>875</v>
@@ -1417,7 +1417,7 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>33619</v>
+        <v>8367</v>
       </c>
       <c r="C58">
         <v>721</v>
@@ -1431,7 +1431,7 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>28558</v>
+        <v>6329</v>
       </c>
       <c r="C59">
         <v>756</v>
@@ -1445,7 +1445,7 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>21924</v>
+        <v>8540</v>
       </c>
       <c r="C60">
         <v>703</v>
@@ -1459,7 +1459,7 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>26747</v>
+        <v>4601</v>
       </c>
       <c r="C61">
         <v>708</v>
@@ -1473,7 +1473,7 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>53322</v>
+        <v>4984</v>
       </c>
       <c r="C62">
         <v>759</v>
@@ -1487,7 +1487,7 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>29591</v>
+        <v>9320</v>
       </c>
       <c r="C63">
         <v>720</v>
@@ -1501,7 +1501,7 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>28426</v>
+        <v>7668</v>
       </c>
       <c r="C64">
         <v>769</v>
@@ -1515,7 +1515,7 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>68303</v>
+        <v>3408</v>
       </c>
       <c r="C65">
         <v>774</v>
@@ -1529,7 +1529,7 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>57022</v>
+        <v>8173</v>
       </c>
       <c r="C66">
         <v>781</v>

</xml_diff>